<commit_message>
Author              :Ashish Mishra Story ID            :SSDMS-42 Files Modified      :AshishMishra.xlsx Description         :Sprint Tracking Sheet modified for task distribution
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AshishMishra.xlsx
+++ b/TeamDetails/TasksBreakDown/AshishMishra.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashish Mishra\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashish Mishra\Desktop\project\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>Story ID</t>
   </si>
@@ -51,31 +51,16 @@
     <t>Story Estimate</t>
   </si>
   <si>
-    <t>SSDMS-37</t>
-  </si>
-  <si>
     <t>T1</t>
   </si>
   <si>
     <t>T2</t>
   </si>
   <si>
-    <t>SSDMS-42</t>
-  </si>
-  <si>
-    <t>Creating necessary Skeleton for making Manage Registration Table</t>
-  </si>
-  <si>
     <t>T3</t>
   </si>
   <si>
-    <t>Creating Division for Manage Registration Table</t>
-  </si>
-  <si>
     <t>T4</t>
-  </si>
-  <si>
-    <t>Creating basic structure of the table</t>
   </si>
   <si>
     <t>T5</t>
@@ -84,25 +69,49 @@
     <t>Labelling Entities using JS</t>
   </si>
   <si>
-    <t>Configuring JDBC connectivity with Database</t>
+    <t>T6</t>
   </si>
   <si>
-    <t>Creating a Dummy DataBase</t>
+    <t>T8</t>
   </si>
   <si>
-    <t>writing files  in eclipse(yml,Configsql,Dto,Dao,Controller,Service)</t>
+    <t>T9</t>
   </si>
   <si>
-    <t>Storing the data in the database</t>
+    <t>SSDMS-37 (Manage Registration)</t>
   </si>
   <si>
-    <t>Review by QA</t>
+    <t>T10</t>
   </si>
   <si>
-    <t>Understanding the why of the story</t>
+    <t>Unit testing</t>
   </si>
   <si>
-    <t>T6</t>
+    <t>Code Review and Incorporate feedback</t>
+  </si>
+  <si>
+    <t>Understand why of the story</t>
+  </si>
+  <si>
+    <t>Create layout of HTML page</t>
+  </si>
+  <si>
+    <t>Createui grid table  for Manage Registration as per GD</t>
+  </si>
+  <si>
+    <t>Edit Icon, approve icon, reject icon</t>
+  </si>
+  <si>
+    <t>Comment box</t>
+  </si>
+  <si>
+    <t>Styleing the layout</t>
+  </si>
+  <si>
+    <t>Create  necessary Skeleton for making Manage Registration Table</t>
+  </si>
+  <si>
+    <t>T11</t>
   </si>
 </sst>
 </file>
@@ -235,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -259,14 +268,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2848,10 +2877,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G48"/>
+  <dimension ref="A2:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2874,9 +2903,7 @@
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2888,18 +2915,17 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="14">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6">
-        <f>SUM(E3:E7)</f>
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -2911,31 +2937,31 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G47" si="0">E4-F4</f>
-        <v>3</v>
+        <f t="shared" ref="G4:G53" si="0">E4-F4</f>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -2947,31 +2973,31 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2983,61 +3009,62 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="6">
-        <f>SUM(E10:E14)</f>
-        <v>4.5</v>
-      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.5</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -3049,13 +3076,13 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -3067,96 +3094,62 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
@@ -3167,8 +3160,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2"/>
@@ -3179,8 +3172,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
       <c r="E21" s="2"/>
@@ -3192,7 +3185,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
@@ -3503,15 +3496,88 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="2"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D55" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="A10:A15"/>
+  <mergeCells count="2">
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="A3:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author :   Ashish mishra Comment :  this is my updated burnt hour in taskbreakdown excel sheet.
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AshishMishra.xlsx
+++ b/TeamDetails/TasksBreakDown/AshishMishra.xlsx
@@ -2879,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" activeCellId="1" sqref="F6 G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2930,10 +2930,12 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
       <c r="G3" s="2">
         <f>E3-F3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2948,10 +2950,12 @@
       <c r="E4" s="2">
         <v>4</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>4</v>
+      </c>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G53" si="0">E4-F4</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2966,10 +2970,12 @@
       <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author      :Ashish Mishra comment : burnt hour updated in AshishMishra.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AshishMishra.xlsx
+++ b/TeamDetails/TasksBreakDown/AshishMishra.xlsx
@@ -2880,7 +2880,7 @@
   <dimension ref="A2:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" activeCellId="1" sqref="F6 G12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2971,11 +2971,11 @@
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2990,10 +2990,12 @@
       <c r="E6" s="2">
         <v>2</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3008,10 +3010,12 @@
       <c r="E7" s="2">
         <v>2</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author            :Ashish Mishra Files Modified    :AshishMishra.xlsx Files Description :Add Total hours and status in the AshishMishra.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AshishMishra.xlsx
+++ b/TeamDetails/TasksBreakDown/AshishMishra.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>Story ID</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>T11</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Done</t>
   </si>
 </sst>
 </file>
@@ -244,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -278,6 +287,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2877,10 +2889,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G55"/>
+  <dimension ref="A2:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2893,7 +2905,7 @@
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2913,12 +2925,15 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="H2" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="15">
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2937,10 +2952,13 @@
         <f>E3-F3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="15"/>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2957,10 +2975,13 @@
         <f t="shared" ref="G4:G53" si="0">E4-F4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="15"/>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2977,10 +2998,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="15"/>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2997,10 +3021,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="15"/>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
@@ -3017,10 +3044,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="15"/>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3036,9 +3066,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="15"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3054,9 +3084,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="15"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3067,9 +3097,9 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="15"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
@@ -3085,9 +3115,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="16"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
@@ -3103,16 +3133,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="10">
+        <v>17</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="2"/>
@@ -3121,7 +3155,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="2"/>
@@ -3130,7 +3164,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
Author         :Ashish Mishra Story ID       :SSDMS-37 files modified :AshishMishra.xlsx Description    :hours burnt updated
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AshishMishra.xlsx
+++ b/TeamDetails/TasksBreakDown/AshishMishra.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
   <si>
     <t>Story ID</t>
   </si>
@@ -2892,7 +2892,7 @@
   <dimension ref="A2:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3060,10 +3060,15 @@
       <c r="E8" s="2">
         <v>1</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3078,10 +3083,15 @@
       <c r="E9" s="2">
         <v>2</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>